<commit_message>
Te quiero idoia Zabalo
</commit_message>
<xml_diff>
--- a/Cert/AMFE-s_Producto_GlaucoTech.xlsx
+++ b/Cert/AMFE-s_Producto_GlaucoTech.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Escritorio\3ºCURSO\2.Cuatri\PBL6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Escritorio\3ºCURSO\2.Cuatri\PBL6\Certif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46FA394-2EB6-41AA-840A-09E22DBB60B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BC9E5BA-C1D8-4418-89EF-EED4F146E55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
   <si>
     <t>EFECTOS</t>
   </si>
@@ -174,21 +174,6 @@
     <t>Desvinculación de la carpeta del paciente con la imagen</t>
   </si>
   <si>
-    <t>ETIQUETA</t>
-  </si>
-  <si>
-    <t>Omisión de información crucial</t>
-  </si>
-  <si>
-    <t>Etiqueta poco clara y difícil de entender</t>
-  </si>
-  <si>
-    <t>Mal estructuramiento y diseño de la información proporcionada en la etiqueta</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elección errónea de la información a añadida</t>
-  </si>
-  <si>
     <t>PÁGINA WEB</t>
   </si>
   <si>
@@ -228,9 +213,6 @@
     <t>Requisito de asignación de nombre a cada imagen insertada en el programa</t>
   </si>
   <si>
-    <t>Responsable de la validación y comprobación del etiquetado final</t>
-  </si>
-  <si>
     <t>Sistema de asistencia al cliente activo y equipo de informatica  encargada del mantenimiento de la página,  para la rapida resolución de los problemas</t>
   </si>
   <si>
@@ -250,12 +232,6 @@
   </si>
   <si>
     <t>La intensidad de las imágenes no es igual que la de las imágenes con las que el modelo predictivo está entrenado</t>
-  </si>
-  <si>
-    <t>Un diseño confuso o desorganizado de la etiqueta  podría llevar a errores en el uso del producto</t>
-  </si>
-  <si>
-    <t>Los usuarios pueden estar en riesgo de usar el producto de manera incorrecta</t>
   </si>
   <si>
     <t>Error en la conexión entre la página web y la base de datos en la que se almacene el software</t>
@@ -865,6 +841,105 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -879,105 +954,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,10 +1459,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:U26"/>
+  <dimension ref="B2:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1516,261 +1492,261 @@
   <sheetData>
     <row r="2" spans="2:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:21" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="33"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="28"/>
     </row>
     <row r="4" spans="2:21" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="36"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="31"/>
     </row>
     <row r="5" spans="2:21" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="39"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="34"/>
     </row>
     <row r="6" spans="2:21" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="59"/>
-      <c r="T6" s="59"/>
-      <c r="U6" s="60"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="55"/>
     </row>
     <row r="7" spans="2:21" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="62"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="63"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="58"/>
     </row>
     <row r="8" spans="2:21" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="56"/>
-      <c r="P8" s="57"/>
-      <c r="Q8" s="45" t="s">
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="47"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="42"/>
     </row>
     <row r="9" spans="2:21" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="56"/>
-      <c r="O9" s="56"/>
-      <c r="P9" s="57"/>
-      <c r="Q9" s="46" t="s">
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="46"/>
-      <c r="U9" s="47"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="42"/>
     </row>
     <row r="10" spans="2:21" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="46" t="s">
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="46"/>
-      <c r="U10" s="47"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="42"/>
     </row>
     <row r="11" spans="2:21" ht="53.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="40" t="s">
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="42" t="s">
+      <c r="P11" s="36"/>
+      <c r="Q11" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="R11" s="43"/>
-      <c r="S11" s="43"/>
-      <c r="T11" s="43"/>
-      <c r="U11" s="44"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="39"/>
     </row>
     <row r="12" spans="2:21" ht="30.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="48" t="s">
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="29" t="s">
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="48" t="s">
+      <c r="P12" s="63"/>
+      <c r="Q12" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="R12" s="49"/>
-      <c r="S12" s="49"/>
-      <c r="T12" s="49"/>
-      <c r="U12" s="50"/>
+      <c r="R12" s="44"/>
+      <c r="S12" s="44"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="45"/>
     </row>
     <row r="13" spans="2:21" ht="70.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="51"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="5" t="s">
         <v>1</v>
       </c>
@@ -1830,17 +1806,17 @@
       </c>
     </row>
     <row r="14" spans="2:21" ht="97.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="59" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F14" s="19">
         <v>8</v>
@@ -1856,7 +1832,7 @@
         <v>288</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="K14" s="23">
         <v>8</v>
@@ -1880,15 +1856,15 @@
       <c r="U14" s="3"/>
     </row>
     <row r="15" spans="2:21" ht="97.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="14" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F15" s="19">
         <v>9</v>
@@ -1900,11 +1876,11 @@
         <v>9</v>
       </c>
       <c r="I15" s="21">
-        <f t="shared" ref="I15:I26" si="0">F15*G15*H15</f>
+        <f t="shared" ref="I15:I24" si="0">F15*G15*H15</f>
         <v>324</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="K15" s="23">
         <v>9</v>
@@ -1916,7 +1892,7 @@
         <v>5</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" ref="N15:N26" si="1">K15*L15*M15</f>
+        <f t="shared" ref="N15:N24" si="1">K15*L15*M15</f>
         <v>90</v>
       </c>
       <c r="O15" s="2"/>
@@ -1928,15 +1904,15 @@
       <c r="U15" s="2"/>
     </row>
     <row r="16" spans="2:21" ht="97.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="27"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F16" s="19">
         <v>7</v>
@@ -1952,7 +1928,7 @@
         <v>210</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K16" s="23">
         <v>7</v>
@@ -1976,15 +1952,15 @@
       <c r="U16" s="2"/>
     </row>
     <row r="17" spans="2:21" ht="97.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="28"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F17" s="19">
         <v>7</v>
@@ -2000,7 +1976,7 @@
         <v>175</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K17" s="23">
         <v>7</v>
@@ -2031,10 +2007,10 @@
         <v>35</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F18" s="20">
         <v>7</v>
@@ -2050,7 +2026,7 @@
         <v>336</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K18" s="20">
         <v>7</v>
@@ -2081,10 +2057,10 @@
         <v>34</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F19" s="19">
         <v>8</v>
@@ -2100,7 +2076,7 @@
         <v>392</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K19" s="23">
         <v>8</v>
@@ -2124,7 +2100,7 @@
       <c r="U19" s="2"/>
     </row>
     <row r="20" spans="2:21" ht="97.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="59" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="14" t="s">
@@ -2150,7 +2126,7 @@
         <v>360</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K20" s="2">
         <v>8</v>
@@ -2174,7 +2150,7 @@
       <c r="U20" s="2"/>
     </row>
     <row r="21" spans="2:21" ht="89.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="28"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="14" t="s">
         <v>41</v>
       </c>
@@ -2198,7 +2174,7 @@
         <v>224</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K21" s="2">
         <v>7</v>
@@ -2222,46 +2198,46 @@
       <c r="U21" s="2"/>
     </row>
     <row r="22" spans="2:21" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="59" t="s">
         <v>44</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="19">
+        <v>45</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="17">
         <v>6</v>
       </c>
       <c r="G22" s="18">
+        <v>4</v>
+      </c>
+      <c r="H22" s="19">
         <v>6</v>
       </c>
-      <c r="H22" s="19">
-        <v>8</v>
-      </c>
-      <c r="I22" s="21">
+      <c r="I22" s="25">
         <f t="shared" si="0"/>
-        <v>288</v>
-      </c>
-      <c r="J22" s="18" t="s">
-        <v>62</v>
+        <v>144</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>57</v>
       </c>
       <c r="K22" s="23">
         <v>6</v>
       </c>
       <c r="L22" s="23">
+        <v>2</v>
+      </c>
+      <c r="M22" s="23">
         <v>4</v>
-      </c>
-      <c r="M22" s="23">
-        <v>3</v>
       </c>
       <c r="N22" s="3">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -2271,45 +2247,45 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
     </row>
-    <row r="23" spans="2:21" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="27"/>
+    <row r="23" spans="2:21" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="60"/>
       <c r="C23" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="19">
-        <v>6</v>
+        <v>58</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="17">
+        <v>8</v>
       </c>
       <c r="G23" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H23" s="19">
+        <v>4</v>
+      </c>
+      <c r="I23" s="25">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="23">
         <v>8</v>
       </c>
-      <c r="I23" s="21">
-        <f t="shared" si="0"/>
-        <v>288</v>
-      </c>
-      <c r="J23" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="K23" s="23">
-        <v>6</v>
-      </c>
       <c r="L23" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M23" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N23" s="3">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -2319,43 +2295,41 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
     </row>
-    <row r="24" spans="2:21" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
-        <v>49</v>
-      </c>
+    <row r="24" spans="2:21" ht="140.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="61"/>
       <c r="C24" s="14" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F24" s="17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G24" s="18">
         <v>4</v>
       </c>
       <c r="H24" s="19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I24" s="25">
         <f t="shared" si="0"/>
-        <v>144</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>63</v>
+        <v>128</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="K24" s="23">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L24" s="23">
         <v>2</v>
       </c>
       <c r="M24" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N24" s="3">
         <f t="shared" si="1"/>
@@ -2369,104 +2343,12 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
     </row>
-    <row r="25" spans="2:21" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
-      <c r="C25" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="17">
-        <v>8</v>
-      </c>
-      <c r="G25" s="18">
-        <v>4</v>
-      </c>
-      <c r="H25" s="19">
-        <v>4</v>
-      </c>
-      <c r="I25" s="25">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="K25" s="23">
-        <v>8</v>
-      </c>
-      <c r="L25" s="23">
-        <v>2</v>
-      </c>
-      <c r="M25" s="23">
-        <v>2</v>
-      </c>
-      <c r="N25" s="3">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-    </row>
-    <row r="26" spans="2:21" ht="140.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="28"/>
-      <c r="C26" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="F26" s="17">
-        <v>8</v>
-      </c>
-      <c r="G26" s="18">
-        <v>4</v>
-      </c>
-      <c r="H26" s="19">
-        <v>4</v>
-      </c>
-      <c r="I26" s="25">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="J26" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="K26" s="23">
-        <v>8</v>
-      </c>
-      <c r="L26" s="23">
-        <v>2</v>
-      </c>
-      <c r="M26" s="23">
-        <v>3</v>
-      </c>
-      <c r="N26" s="3">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="O12:P12"/>
     <mergeCell ref="B3:U5"/>
     <mergeCell ref="O11:P11"/>
     <mergeCell ref="Q11:U11"/>
@@ -2483,11 +2365,6 @@
     <mergeCell ref="B11:N11"/>
     <mergeCell ref="B6:U6"/>
     <mergeCell ref="B7:U7"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="O12:P12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="34" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -2511,23 +2388,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a60bd0ed-6c94-4ccf-b866-c76c7887cd60" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004CFD171F51FA73478CA9FE425E910C9D" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="65efb9c71fa12a42015e1712bef1605a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a60bd0ed-6c94-4ccf-b866-c76c7887cd60" xmlns:ns4="97b8de9a-07de-4d8c-840a-97ec8fb03718" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f8c8a9d5849dce9e7dd468bec265966d" ns3:_="" ns4:_="">
     <xsd:import namespace="a60bd0ed-6c94-4ccf-b866-c76c7887cd60"/>
@@ -2748,32 +2608,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBD84341-9A91-49B0-9AA3-6A47683F30F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="97b8de9a-07de-4d8c-840a-97ec8fb03718"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a60bd0ed-6c94-4ccf-b866-c76c7887cd60"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{307E8AEE-8FE2-4BC2-93C3-67C7900A28EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a60bd0ed-6c94-4ccf-b866-c76c7887cd60" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39EB5903-899A-428A-A62F-8CB4DA68C706}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2790,4 +2642,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{307E8AEE-8FE2-4BC2-93C3-67C7900A28EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBD84341-9A91-49B0-9AA3-6A47683F30F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="97b8de9a-07de-4d8c-840a-97ec8fb03718"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a60bd0ed-6c94-4ccf-b866-c76c7887cd60"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>